<commit_message>
& - 24078 от 28.11.2025 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/France/#EURO#France#Commemorative#[2007-present]#UNC.xlsx
+++ b/Collections/EURO/France/#EURO#France#Commemorative#[2007-present]#UNC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\France\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCDEA1A-1CAC-49D4-9A52-C40E9CABC7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE04A66B-DB9A-4FDF-81C6-E547DB800EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -141,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="109">
   <si>
     <t>Year</t>
   </si>
@@ -463,6 +466,12 @@
   </si>
   <si>
     <t>Subtype_5#Coloured</t>
+  </si>
+  <si>
+    <t>Notre-Dame de Paris Cathedral</t>
+  </si>
+  <si>
+    <t>20.000.000</t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1291,10 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2576,7 +2585,9 @@
       <c r="A44" s="5">
         <v>2025</v>
       </c>
-      <c r="B44" s="6"/>
+      <c r="B44" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
         <v>38</v>
@@ -2584,10 +2595,14 @@
       <c r="E44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="G44" s="7"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="24">
+      <c r="H44" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I44" s="8">
         <v>1</v>
       </c>
       <c r="J44" s="9" t="str">
@@ -2613,12 +2628,12 @@
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="I3 I6 I10 I12 I14 I17 I23 I26 I8 I21">
-    <cfRule type="containsText" dxfId="27" priority="85" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="27" priority="87" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6 I3 I10 I12 I14 I17 I23 I26 I8 I21">
-    <cfRule type="colorScale" priority="86">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2630,12 +2645,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7 I11 I13 I16 I19 I22 I25 I28 I30">
-    <cfRule type="containsText" dxfId="26" priority="77" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="26" priority="79" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11 I7 I13 I16 I19 I22 I25 I28 I30">
-    <cfRule type="colorScale" priority="78">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2647,11 +2662,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="containsText" dxfId="25" priority="65" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="25" priority="67" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I5))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="containsText" dxfId="24" priority="65" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2663,13 +2695,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="24" priority="63" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="colorScale" priority="64">
+  <conditionalFormatting sqref="I18">
+    <cfRule type="containsText" dxfId="23" priority="61" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2680,12 +2712,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="23" priority="59" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="I20">
+    <cfRule type="containsText" dxfId="22" priority="59" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="containsText" dxfId="21" priority="57" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2697,17 +2734,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="22" priority="57" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="containsText" dxfId="21" priority="55" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I24))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2719,7 +2746,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
+  <conditionalFormatting sqref="I27">
+    <cfRule type="containsText" dxfId="20" priority="55" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2731,12 +2763,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="containsText" dxfId="20" priority="53" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I27))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
+  <conditionalFormatting sqref="I31">
+    <cfRule type="containsText" dxfId="19" priority="53" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2748,13 +2780,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="19" priority="51" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I31))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="colorScale" priority="52">
+  <conditionalFormatting sqref="I38">
+    <cfRule type="containsText" dxfId="18" priority="31" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I38))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2765,12 +2797,80 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I38))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I29">
+    <cfRule type="containsText" dxfId="17" priority="47" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="containsText" dxfId="16" priority="45" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="containsText" dxfId="15" priority="43" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="containsText" dxfId="14" priority="39" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I35))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="containsText" dxfId="13" priority="29" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I39))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2782,13 +2882,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="17" priority="45" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="colorScale" priority="46">
+  <conditionalFormatting sqref="I36">
+    <cfRule type="containsText" dxfId="12" priority="35" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I36))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2799,13 +2899,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="16" priority="43" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="colorScale" priority="44">
+  <conditionalFormatting sqref="I37">
+    <cfRule type="containsText" dxfId="11" priority="33" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I37))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2816,46 +2916,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="15" priority="41" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I33))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="14" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="containsText" dxfId="13" priority="27" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I39))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I34">
+    <cfRule type="containsText" dxfId="10" priority="27" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I34))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2867,13 +2933,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="containsText" dxfId="12" priority="33" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I36))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="I40">
+    <cfRule type="containsText" dxfId="9" priority="23" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I40))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2884,46 +2950,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="containsText" dxfId="11" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I37))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="10" priority="25" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I34))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="containsText" dxfId="9" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I40))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
+  <conditionalFormatting sqref="I9">
+    <cfRule type="containsText" dxfId="8" priority="21" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2935,12 +2967,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
+  <conditionalFormatting sqref="I4">
+    <cfRule type="containsText" dxfId="7" priority="19" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2952,13 +2984,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="containsText" dxfId="7" priority="17" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="I41">
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I41))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2969,12 +3001,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I41))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
+  <conditionalFormatting sqref="I42">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I42))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2986,30 +3018,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I42))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I43))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>

</xml_diff>